<commit_message>
Username & Password variants
</commit_message>
<xml_diff>
--- a/TestCase.xlsx
+++ b/TestCase.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -486,12 +486,33 @@
           <t>TC001</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr"/>
-      <c r="C2" t="inlineStr"/>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Gốc</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Gốc</t>
+        </is>
+      </c>
       <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>tomsmith / SuperSecretPassword!</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>You logged into a secure area!
+×</t>
+        </is>
+      </c>
       <c r="H2" t="inlineStr">
         <is>
           <t>Pass</t>
@@ -505,12 +526,33 @@
           <t>TC002</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr"/>
-      <c r="C3" t="inlineStr"/>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Tất cả viết thường</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Tất cả viết thường</t>
+        </is>
+      </c>
       <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>tomsmith / SuperSecretPassword!</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>You logged into a secure area!
+×</t>
+        </is>
+      </c>
       <c r="H3" t="inlineStr">
         <is>
           <t>Pass</t>
@@ -524,18 +566,644 @@
           <t>TC003</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr"/>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Tất cả viết hoa</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Tất cả viết hoa</t>
+        </is>
+      </c>
       <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>TOMSMITH / SuperSecretPassword!</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
       <c r="H4" t="inlineStr">
         <is>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>TC004</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Khoảng trắng ở cuối</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Khoảng trắng ở cuối</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>tomsmith  / SuperSecretPassword!</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>TC005</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Khoảng trắng ở đầu</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Khoảng trắng ở đầu</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> tomsmith / SuperSecretPassword!</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>TC006</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Viết hoa chữ cái đầu</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Viết hoa chữ cái đầu</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Tomsmith / SuperSecretPassword!</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>TC007</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Đảo hoa-thường</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Đảo hoa-thường</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>TOMSMITH / SuperSecretPassword!</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>TC008</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Ký tự xuống dòng ở cuối</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Ký tự xuống dòng ở cuối</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>tomsmith
+ / SuperSecretPassword!</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Message: stale element reference: stale element not found
+  (Session info: chrome=137.0.7151.68); For documentation on this error, please visit: https://www.selenium.dev/documentation/webdriver/troubleshooting/errors#stale-element-reference-exception
+Stacktrace:
+	GetHandleVerifier [0x0xee3763+63299]
+	GetHandleVerifier [0x0xee37a4+63364]
+	(No symbol) [0x0xd11113]
+	(No symbol) [0x0xd22c01]
+	(No symbol) [0x0xd21ce0]
+	(No symbol) [0x0xd183d2]
+	(No symbol) [0x0xd168d1]
+	(No symbol) [0x0xd19c4a]
+	(No symbol) [0x0xd19cc7]
+	(No symbol) [0x0xd5a51a]
+	(No symbol) [0x0xd5a5a1]
+	(No symbol) [0x0xd51fd4]
+	(No symbol) [0x0xd7e57c]
+	(No symbol) [0x0xd4eed4]
+	(No symbol) [0x0xd7e7f4]
+	(No symbol) [0x0xd9fa4a]
+	(No symbol) [0x0xd7e376]
+	(No symbol) [0x0xd4d6e0]
+	(No symbol) [0x0xd4e544]
+	GetHandleVerifier [0x0x113e033+2531347]
+	GetHandleVerifier [0x0x1139332+2511634]
+	GetHandleVerifier [0x0xf09eda+220858]
+	GetHandleVerifier [0x0xefa528+156936]
+	GetHandleVerifier [0x0xf00c5d+183357]
+	GetHandleVerifier [0x0xeeb6c8+95912]
+	GetHandleVerifier [0x0xeeb870+96336]
+	GetHandleVerifier [0x0xed664a+9770]
+	BaseThreadInitThunk [0x0x76a15d49+25]
+	RtlInitializeExceptionChain [0x0x76edd03b+107]
+	RtlGetAppContainerNamedObjectPath [0x0x76edcfc1+561]</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>TC009</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Ký tự tab ở cuối</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Ký tự tab ở cuối</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>tomsmith	 / SuperSecretPassword!</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>You logged into a secure area!
+×</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
           <t>Pass</t>
         </is>
       </c>
-      <c r="I4" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>TC010</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Tất cả viết thường</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Tất cả viết thường</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>tomsmith / supersecretpassword!</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>TC011</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Tất cả viết hoa</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Tất cả viết hoa</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>tomsmith / SUPERSECRETPASSWORD!</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>TC012</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Khoảng trắng ở cuối</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Khoảng trắng ở cuối</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">tomsmith / SuperSecretPassword! </t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>TC013</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Khoảng trắng ở đầu</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Khoảng trắng ở đầu</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>tomsmith /  SuperSecretPassword!</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>TC014</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Viết hoa chữ cái đầu</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Viết hoa chữ cái đầu</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>tomsmith / Supersecretpassword!</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>TC015</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Đảo hoa-thường</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Đảo hoa-thường</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr"/>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>tomsmith / sUPERsECRETpASSWORD!</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>TC016</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Ký tự xuống dòng ở cuối</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Ký tự xuống dòng ở cuối</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr"/>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t xml:space="preserve">tomsmith / SuperSecretPassword!
+</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Message: no such element: Unable to locate element: {"method":"css selector","selector":"button[type='submit']"}
+  (Session info: chrome=137.0.7151.68); For documentation on this error, please visit: https://www.selenium.dev/documentation/webdriver/troubleshooting/errors#no-such-element-exception
+Stacktrace:
+	GetHandleVerifier [0x0xee3763+63299]
+	GetHandleVerifier [0x0xee37a4+63364]
+	(No symbol) [0x0xd11113]
+	(No symbol) [0x0xd5987e]
+	(No symbol) [0x0xd59c1b]
+	(No symbol) [0x0xda2212]
+	(No symbol) [0x0xd7e5c4]
+	(No symbol) [0x0xd9fa4a]
+	(No symbol) [0x0xd7e376]
+	(No symbol) [0x0xd4d6e0]
+	(No symbol) [0x0xd4e544]
+	GetHandleVerifier [0x0x113e033+2531347]
+	GetHandleVerifier [0x0x1139332+2511634]
+	GetHandleVerifier [0x0xf09eda+220858]
+	GetHandleVerifier [0x0xefa528+156936]
+	GetHandleVerifier [0x0xf00c5d+183357]
+	GetHandleVerifier [0x0xeeb6c8+95912]
+	GetHandleVerifier [0x0xeeb870+96336]
+	GetHandleVerifier [0x0xed664a+9770]
+	BaseThreadInitThunk [0x0x76a15d49+25]
+	RtlInitializeExceptionChain [0x0x76edd03b+107]
+	RtlGetAppContainerNamedObjectPath [0x0x76edcfc1+561]</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>TC017</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Ký tự tab ở cuối</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Ký tự tab ở cuối</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr"/>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t xml:space="preserve">tomsmith / SuperSecretPassword!	</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>You logged into a secure area!
+×</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Slightly fixed Auto report writing
</commit_message>
<xml_diff>
--- a/TestCase.xlsx
+++ b/TestCase.xlsx
@@ -500,13 +500,12 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Pass</t>
+          <t>Login Successfully</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>You logged into a secure area!
-×</t>
+          <t>Login Successfully</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -536,13 +535,12 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Pass</t>
+          <t>Login Successfully</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>You logged into a secure area!
-×</t>
+          <t>Login Successfully</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -572,18 +570,17 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Fail</t>
+          <t>Login Fail</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Your username is invalid!
-×</t>
+          <t>Login Fail</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Fail</t>
+          <t>Pass</t>
         </is>
       </c>
       <c r="I4" t="inlineStr"/>
@@ -608,18 +605,17 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Fail</t>
+          <t>Login Fail</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Your username is invalid!
-×</t>
+          <t>Login Fail</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Fail</t>
+          <t>Pass</t>
         </is>
       </c>
       <c r="I5" t="inlineStr"/>
@@ -644,18 +640,17 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Fail</t>
+          <t>Login Fail</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Your username is invalid!
-×</t>
+          <t>Login Fail</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Fail</t>
+          <t>Pass</t>
         </is>
       </c>
       <c r="I6" t="inlineStr"/>
@@ -680,18 +675,17 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Fail</t>
+          <t>Login Fail</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Your username is invalid!
-×</t>
+          <t>Login Fail</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Fail</t>
+          <t>Pass</t>
         </is>
       </c>
       <c r="I7" t="inlineStr"/>
@@ -716,18 +710,17 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Fail</t>
+          <t>Login Fail</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Your username is invalid!
-×</t>
+          <t>Login Fail</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Fail</t>
+          <t>Pass</t>
         </is>
       </c>
       <c r="I8" t="inlineStr"/>
@@ -752,18 +745,17 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Fail</t>
+          <t>Login Fail</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Your password is invalid!
-×</t>
+          <t>Login Fail</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Fail</t>
+          <t>Pass</t>
         </is>
       </c>
       <c r="I9" t="inlineStr"/>
@@ -788,18 +780,17 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Fail</t>
+          <t>Login Fail</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Your password is invalid!
-×</t>
+          <t>Login Fail</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Fail</t>
+          <t>Pass</t>
         </is>
       </c>
       <c r="I10" t="inlineStr"/>
@@ -824,18 +815,17 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Fail</t>
+          <t>Login Fail</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Your password is invalid!
-×</t>
+          <t>Login Fail</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Fail</t>
+          <t>Pass</t>
         </is>
       </c>
       <c r="I11" t="inlineStr"/>
@@ -860,18 +850,17 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Fail</t>
+          <t>Login Fail</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Your password is invalid!
-×</t>
+          <t>Login Fail</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Fail</t>
+          <t>Pass</t>
         </is>
       </c>
       <c r="I12" t="inlineStr"/>
@@ -896,18 +885,17 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Fail</t>
+          <t>Login Fail</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Your password is invalid!
-×</t>
+          <t>Login Fail</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Fail</t>
+          <t>Pass</t>
         </is>
       </c>
       <c r="I13" t="inlineStr"/>
@@ -932,18 +920,17 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Fail</t>
+          <t>Login Fail</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Your password is invalid!
-×</t>
+          <t>Login Fail</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Fail</t>
+          <t>Pass</t>
         </is>
       </c>
       <c r="I14" t="inlineStr"/>
@@ -968,18 +955,17 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Fail</t>
+          <t>Login Fail</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Your username is invalid!
-×</t>
+          <t>Login Fail</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Fail</t>
+          <t>Pass</t>
         </is>
       </c>
       <c r="I15" t="inlineStr"/>
@@ -1004,18 +990,17 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Fail</t>
+          <t>Login Fail</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>Your password is invalid!
-×</t>
+          <t>Login Fail</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Fail</t>
+          <t>Pass</t>
         </is>
       </c>
       <c r="I16" t="inlineStr"/>
@@ -1040,18 +1025,17 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Fail</t>
+          <t>Login Fail</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>Your username is invalid!
-×</t>
+          <t>Login Fail</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>Fail</t>
+          <t>Pass</t>
         </is>
       </c>
       <c r="I17" t="inlineStr"/>
@@ -1076,18 +1060,17 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Fail</t>
+          <t>Login Fail</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Your username is invalid!
-×</t>
+          <t>Login Fail</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Fail</t>
+          <t>Pass</t>
         </is>
       </c>
       <c r="I18" t="inlineStr"/>
@@ -1112,18 +1095,17 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Fail</t>
+          <t>Login Fail</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>Your username is invalid!
-×</t>
+          <t>Login Fail</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Fail</t>
+          <t>Pass</t>
         </is>
       </c>
       <c r="I19" t="inlineStr"/>
@@ -1148,18 +1130,17 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Fail</t>
+          <t>Login Fail</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>Your username is invalid!
-×</t>
+          <t>Login Fail</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Fail</t>
+          <t>Pass</t>
         </is>
       </c>
       <c r="I20" t="inlineStr"/>
@@ -1184,18 +1165,17 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Fail</t>
+          <t>Login Fail</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>Your username is invalid!
-×</t>
+          <t>Login Fail</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Fail</t>
+          <t>Pass</t>
         </is>
       </c>
       <c r="I21" t="inlineStr"/>
@@ -1220,18 +1200,17 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Fail</t>
+          <t>Login Fail</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>Your username is invalid!
-×</t>
+          <t>Login Fail</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Fail</t>
+          <t>Pass</t>
         </is>
       </c>
       <c r="I22" t="inlineStr"/>

</xml_diff>